<commit_message>
some more code optimization
</commit_message>
<xml_diff>
--- a/src/test/java/com/incubyte/testData/TestData.xlsx
+++ b/src/test/java/com/incubyte/testData/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -245,6 +245,30 @@
   </si>
   <si>
     <t>N+Dpv8$HjJ,</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Torres</t>
+  </si>
+  <si>
+    <t>robert.torres1735829893157@webmail.com</t>
+  </si>
+  <si>
+    <t>^5r39VN'Ub</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>andrew.williams1735829998241@test.com</t>
+  </si>
+  <si>
+    <t>5xX$H^{-t</t>
   </si>
 </sst>
 </file>
@@ -645,16 +669,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F2" s="1"/>
     </row>

</xml_diff>